<commit_message>
Stats: Bugfixes and first successful runs
</commit_message>
<xml_diff>
--- a/stats/Statistics.xlsx
+++ b/stats/Statistics.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lubo9\Desktop\Workspace\ddminj\stats\"/>
     </mc:Choice>
@@ -15,10 +15,12 @@
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
     <sheet name="Template" sheetId="1" r:id="rId2"/>
+    <sheet name="20230426_162906" r:id="rId7" sheetId="3"/>
+    <sheet name="20230426_163105" r:id="rId8" sheetId="4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
   <si>
     <t>GraphTestExecutor</t>
   </si>
@@ -148,12 +150,43 @@
   </si>
   <si>
     <t>Active Reduction</t>
+  </si>
+  <si>
+    <t>C:\Users\lubo9\Desktop\Workspace\ddminj\CalculatorExample</t>
+  </si>
+  <si>
+    <t>src</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>calculator.CalculatorTest#testCalculator</t>
+  </si>
+  <si>
+    <t>org.opentest4j.AssertionFailedError: Unexpected exception type thrown, expected: &lt;calculator.DividedByZeroException&gt; but was: &lt;java.lang.ArithmeticException&gt;</t>
+  </si>
+  <si>
+    <t>IN_MEMORY</t>
+  </si>
+  <si>
+    <t>INFO</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -542,14 +575,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="39.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="30.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -738,13 +771,13 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32"/>
-      <c r="D32">
+      <c r="D32" t="n">
         <f>B32-C32</f>
-        <v>0</v>
-      </c>
-      <c r="G32">
+        <v>0.0</v>
+      </c>
+      <c r="G32" t="n">
         <f>E32-F32</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -775,4 +808,746 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{673030EE-DA1B-46C6-86E3-B27F20851DB4}">
+  <dimension ref="A1:J38"/>
+  <sheetViews>
+    <sheetView tabSelected="false" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="39.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="30.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="n">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="n">
+        <v>33.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="n">
+        <v>322.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" t="n">
+        <v>322.0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="D32" t="n">
+        <f>B32-C32</f>
+        <v>9.0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="G32" t="n">
+        <f>E32-F32</f>
+        <v>9.0</v>
+      </c>
+      <c r="J32" t="n">
+        <v>2932.0</v>
+      </c>
+    </row>
+    <row r="33" ht="15.0" customHeight="true">
+      <c r="A33" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <f>B33-C33</f>
+        <v>8.0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <f>E33-F33</f>
+        <v>17.0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>367.0</v>
+      </c>
+    </row>
+    <row r="34" ht="15.0" customHeight="true">
+      <c r="A34" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <f>B34-C34</f>
+        <v>0.0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <f>E34-F34</f>
+        <v>17.0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>235.0</v>
+      </c>
+    </row>
+    <row r="35" ht="15.0" customHeight="true">
+      <c r="A35" s="0"/>
+      <c r="D35" s="0" t="n">
+        <f>B35-C35</f>
+        <v>0.0</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <f>E35-F35</f>
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36"/>
+      <c r="B36"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37"/>
+      <c r="B37"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38"/>
+      <c r="B38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{673030EE-DA1B-46C6-86E3-B27F20851DB4}">
+  <dimension ref="A1:J38"/>
+  <sheetViews>
+    <sheetView tabSelected="false" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="39.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="30.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="n">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="n">
+        <v>33.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="n">
+        <v>322.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" t="n">
+        <v>322.0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="D32" t="n">
+        <f>B32-C32</f>
+        <v>9.0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="G32" t="n">
+        <f>E32-F32</f>
+        <v>9.0</v>
+      </c>
+      <c r="J32" t="n">
+        <v>2830.0</v>
+      </c>
+    </row>
+    <row r="33" ht="15.0" customHeight="true">
+      <c r="A33" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <f>B33-C33</f>
+        <v>8.0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <f>E33-F33</f>
+        <v>8.0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>361.0</v>
+      </c>
+    </row>
+    <row r="34" ht="15.0" customHeight="true">
+      <c r="A34" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <f>B34-C34</f>
+        <v>0.0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <f>E34-F34</f>
+        <v>0.0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>639.0</v>
+      </c>
+    </row>
+    <row r="35" ht="15.0" customHeight="true">
+      <c r="A35" s="0"/>
+      <c r="D35" s="0" t="n">
+        <f>B35-C35</f>
+        <v>0.0</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <f>E35-F35</f>
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36"/>
+      <c r="B36"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37"/>
+      <c r="B37"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38"/>
+      <c r="B38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Stats: Full HDDrec tracking
</commit_message>
<xml_diff>
--- a/stats/Statistics.xlsx
+++ b/stats/Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lubo9\Desktop\Workspace\ddminj\stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6039512C-7A15-4EFB-901B-029ABD62545E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37A66CB-5D2B-4FBA-B0E9-15B7BF3A2C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-26385" yWindow="5070" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{76C4E7CE-BBFA-4642-BC60-85888EE16FB5}"/>
   </bookViews>
@@ -513,7 +513,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49983D61-AF81-4DD3-A0DE-F69ED8BC4136}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181B9FD2-3598-489A-A248-003383B0482A}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -533,7 +533,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF2C7062-5792-4119-BC20-0743C61FB557}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E818E1-B328-405D-B8AC-B8E5F8AB6EF6}">
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>

<commit_message>
Stats: first run with tracker on server cont
</commit_message>
<xml_diff>
--- a/stats/Statistics.xlsx
+++ b/stats/Statistics.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lubo9\Desktop\Workspace\ddminj\stats\"/>
     </mc:Choice>
@@ -15,10 +15,11 @@
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
     <sheet name="Template" sheetId="1" r:id="rId2"/>
+    <sheet name="HDD__20230427_155542" r:id="rId7" sheetId="3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <t>Execution Time (ms)</t>
   </si>
@@ -172,12 +173,88 @@
   </si>
   <si>
     <t>ALGORITHM</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>/home/lukasbosshart/workspace/defects4j/bugs/csv_4_b/</t>
+  </si>
+  <si>
+    <t>src/main/java</t>
+  </si>
+  <si>
+    <t>src/test/java</t>
+  </si>
+  <si>
+    <t>org.apache.commons.csv.CSVParserTest#testNoHeaderMap</t>
+  </si>
+  <si>
+    <t>java.lang.NullPointerException</t>
+  </si>
+  <si>
+    <t>IN_MEMORY</t>
+  </si>
+  <si>
+    <t>INFO</t>
+  </si>
+  <si>
+    <t>HDD</t>
+  </si>
+  <si>
+    <t>0-0</t>
+  </si>
+  <si>
+    <t>0-1</t>
+  </si>
+  <si>
+    <t>0-2</t>
+  </si>
+  <si>
+    <t>0-3</t>
+  </si>
+  <si>
+    <t>0-4</t>
+  </si>
+  <si>
+    <t>0-5</t>
+  </si>
+  <si>
+    <t>0-6</t>
+  </si>
+  <si>
+    <t>0-7</t>
+  </si>
+  <si>
+    <t>0-8</t>
+  </si>
+  <si>
+    <t>0-9</t>
+  </si>
+  <si>
+    <t>0-10</t>
+  </si>
+  <si>
+    <t>0-11</t>
+  </si>
+  <si>
+    <t>0-12</t>
+  </si>
+  <si>
+    <t>0-13</t>
+  </si>
+  <si>
+    <t>0-14</t>
+  </si>
+  <si>
+    <t>0-15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -736,6 +813,423 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EB3A-4356-BAD6-BBDF08267E46}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1714316624"/>
+        <c:axId val="1714318064"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1714316624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># compiler calls</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1714318064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1714318064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># fragments</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1714316624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t># of fragments after # of compiler calls</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Template!$F$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Result</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>HDD__20230427_155542!$J$32:$J$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>HDD__20230427_155542!$F$32:$F$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1652,6 +2146,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1957,7 +2494,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.5703125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1985,14 +2522,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="39.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="30.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2104,9 +2641,9 @@
       <c r="C20" t="s">
         <v>35</v>
       </c>
-      <c r="D20">
+      <c r="D20" t="n">
         <f>COUNTA(A32:A32)</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2222,21 +2759,21 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32"/>
-      <c r="D32">
+      <c r="D32" t="n">
         <f>B32-C32</f>
-        <v>0</v>
-      </c>
-      <c r="G32">
+        <v>0.0</v>
+      </c>
+      <c r="G32" t="n">
         <f>E32-F32</f>
-        <v>0</v>
-      </c>
-      <c r="J32">
+        <v>0.0</v>
+      </c>
+      <c r="J32" t="n">
         <f>SUM($H$32:H32)</f>
-        <v>0</v>
-      </c>
-      <c r="K32">
+        <v>0.0</v>
+      </c>
+      <c r="K32" t="n">
         <f>SUM($I$32:I32)</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2268,4 +2805,1000 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1358C94B-32D6-4385-8263-23B281415B45}">
+  <dimension ref="A1:L47"/>
+  <sheetViews>
+    <sheetView tabSelected="false" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="39.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="30.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="n">
+        <v>5118.0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="n">
+        <f>COUNTA(A32:A47)</f>
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="n">
+        <v>88079.0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="n">
+        <f>B27/D20</f>
+        <v>4344.4375</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="n">
+        <v>2917.0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="4" t="n">
+        <f>(B20-B23)/B20</f>
+        <v>0.6162563501367722</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1964.0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="4" t="n">
+        <f>D22/D20</f>
+        <v>0.03851602188354826</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="n">
+        <v>15468.0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" t="str">
+        <f>TEXT(B26/86400000,"hh:mm:ss.000")</f>
+        <v>00:07:49.092</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="n">
+        <v>737.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="n">
+        <v>469092.0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="n">
+        <v>69511.0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="n">
+        <v>902.0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D32" t="n">
+        <f>B32-C32</f>
+        <v>0.0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>5118.0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>5118.0</v>
+      </c>
+      <c r="G32" t="n">
+        <f>E32-F32</f>
+        <v>0.0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J32" t="n">
+        <f>SUM($H$32:H32)</f>
+        <v>26.0</v>
+      </c>
+      <c r="K32" t="n">
+        <f>SUM($I$32:I32)</f>
+        <v>1.0</v>
+      </c>
+      <c r="L32" t="n">
+        <v>3808.0</v>
+      </c>
+    </row>
+    <row r="33" ht="15.0" customHeight="true">
+      <c r="A33" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" t="n">
+        <v>83.0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>83.0</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <f>B33-C33</f>
+        <v>0.0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>5118.0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>5118.0</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <f>E33-F33</f>
+        <v>0.0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>209.0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <f>SUM($H$32:H33)</f>
+        <v>235.0</v>
+      </c>
+      <c r="K33" s="0" t="n">
+        <f>SUM($I$32:I33)</f>
+        <v>1.0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>7450.0</v>
+      </c>
+    </row>
+    <row r="34" ht="15.0" customHeight="true">
+      <c r="A34" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" t="n">
+        <v>639.0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>550.0</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <f>B34-C34</f>
+        <v>89.0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>5118.0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>4248.0</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <f>E34-F34</f>
+        <v>870.0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>15861.0</v>
+      </c>
+      <c r="I34" t="n">
+        <v>89.0</v>
+      </c>
+      <c r="J34" s="0" t="n">
+        <f>SUM($H$32:H34)</f>
+        <v>16096.0</v>
+      </c>
+      <c r="K34" s="0" t="n">
+        <f>SUM($I$32:I34)</f>
+        <v>90.0</v>
+      </c>
+      <c r="L34" t="n">
+        <v>217958.0</v>
+      </c>
+    </row>
+    <row r="35" ht="15.0" customHeight="true">
+      <c r="A35" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" t="n">
+        <v>795.0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>603.0</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <f>B35-C35</f>
+        <v>192.0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>4248.0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>4056.0</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <f>E35-F35</f>
+        <v>192.0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>41920.0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>598.0</v>
+      </c>
+      <c r="J35" s="0" t="n">
+        <f>SUM($H$32:H35)</f>
+        <v>58016.0</v>
+      </c>
+      <c r="K35" s="0" t="n">
+        <f>SUM($I$32:I35)</f>
+        <v>688.0</v>
+      </c>
+      <c r="L35" t="n">
+        <v>130337.0</v>
+      </c>
+    </row>
+    <row r="36" ht="15.0" customHeight="true">
+      <c r="A36" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" t="n">
+        <v>339.0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>169.0</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <f>B36-C36</f>
+        <v>170.0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>4056.0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>2248.0</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <f>E36-F36</f>
+        <v>1808.0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>6397.0</v>
+      </c>
+      <c r="I36" t="n">
+        <v>144.0</v>
+      </c>
+      <c r="J36" s="0" t="n">
+        <f>SUM($H$32:H36)</f>
+        <v>64413.0</v>
+      </c>
+      <c r="K36" s="0" t="n">
+        <f>SUM($I$32:I36)</f>
+        <v>832.0</v>
+      </c>
+      <c r="L36" t="n">
+        <v>65906.0</v>
+      </c>
+    </row>
+    <row r="37" ht="15.0" customHeight="true">
+      <c r="A37" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" t="n">
+        <v>154.0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>134.0</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <f>B37-C37</f>
+        <v>20.0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>2248.0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>2202.0</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <f>E37-F37</f>
+        <v>46.0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>1409.0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="J37" s="0" t="n">
+        <f>SUM($H$32:H37)</f>
+        <v>65822.0</v>
+      </c>
+      <c r="K37" s="0" t="n">
+        <f>SUM($I$32:I37)</f>
+        <v>852.0</v>
+      </c>
+      <c r="L37" t="n">
+        <v>7650.0</v>
+      </c>
+    </row>
+    <row r="38" ht="15.0" customHeight="true">
+      <c r="A38" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>242.0</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <f>B38-C38</f>
+        <v>14.0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>2202.0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>2038.0</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <f>E38-F38</f>
+        <v>164.0</v>
+      </c>
+      <c r="H38" t="n">
+        <v>2733.0</v>
+      </c>
+      <c r="I38" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="J38" s="0" t="n">
+        <f>SUM($H$32:H38)</f>
+        <v>68555.0</v>
+      </c>
+      <c r="K38" s="0" t="n">
+        <f>SUM($I$32:I38)</f>
+        <v>876.0</v>
+      </c>
+      <c r="L38" t="n">
+        <v>27912.0</v>
+      </c>
+    </row>
+    <row r="39" ht="15.0" customHeight="true">
+      <c r="A39" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" t="n">
+        <v>85.0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>81.0</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <f>B39-C39</f>
+        <v>4.0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>2038.0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>2027.0</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <f>E39-F39</f>
+        <v>11.0</v>
+      </c>
+      <c r="H39" t="n">
+        <v>505.0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="J39" s="0" t="n">
+        <f>SUM($H$32:H39)</f>
+        <v>69060.0</v>
+      </c>
+      <c r="K39" s="0" t="n">
+        <f>SUM($I$32:I39)</f>
+        <v>882.0</v>
+      </c>
+      <c r="L39" t="n">
+        <v>2536.0</v>
+      </c>
+    </row>
+    <row r="40" ht="15.0" customHeight="true">
+      <c r="A40" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <f>B40-C40</f>
+        <v>2.0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>2027.0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>2025.0</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <f>E40-F40</f>
+        <v>2.0</v>
+      </c>
+      <c r="H40" t="n">
+        <v>191.0</v>
+      </c>
+      <c r="I40" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J40" s="0" t="n">
+        <f>SUM($H$32:H40)</f>
+        <v>69251.0</v>
+      </c>
+      <c r="K40" s="0" t="n">
+        <f>SUM($I$32:I40)</f>
+        <v>885.0</v>
+      </c>
+      <c r="L40" t="n">
+        <v>1032.0</v>
+      </c>
+    </row>
+    <row r="41" ht="15.0" customHeight="true">
+      <c r="A41" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <f>B41-C41</f>
+        <v>6.0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>2025.0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>1971.0</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <f>E41-F41</f>
+        <v>54.0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>175.0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="J41" s="0" t="n">
+        <f>SUM($H$32:H41)</f>
+        <v>69426.0</v>
+      </c>
+      <c r="K41" s="0" t="n">
+        <f>SUM($I$32:I41)</f>
+        <v>895.0</v>
+      </c>
+      <c r="L41" t="n">
+        <v>1531.0</v>
+      </c>
+    </row>
+    <row r="42" ht="15.0" customHeight="true">
+      <c r="A42" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <f>B42-C42</f>
+        <v>3.0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>1971.0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>1968.0</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <f>E42-F42</f>
+        <v>3.0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="I42" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J42" s="0" t="n">
+        <f>SUM($H$32:H42)</f>
+        <v>69463.0</v>
+      </c>
+      <c r="K42" s="0" t="n">
+        <f>SUM($I$32:I42)</f>
+        <v>898.0</v>
+      </c>
+      <c r="L42" t="n">
+        <v>588.0</v>
+      </c>
+    </row>
+    <row r="43" ht="15.0" customHeight="true">
+      <c r="A43" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <f>B43-C43</f>
+        <v>2.0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>1968.0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>1966.0</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <f>E43-F43</f>
+        <v>2.0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="I43" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J43" s="0" t="n">
+        <f>SUM($H$32:H43)</f>
+        <v>69500.0</v>
+      </c>
+      <c r="K43" s="0" t="n">
+        <f>SUM($I$32:I43)</f>
+        <v>901.0</v>
+      </c>
+      <c r="L43" t="n">
+        <v>528.0</v>
+      </c>
+    </row>
+    <row r="44" ht="15.0" customHeight="true">
+      <c r="A44" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C44" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <f>B44-C44</f>
+        <v>0.0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1966.0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1966.0</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <f>E44-F44</f>
+        <v>0.0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J44" s="0" t="n">
+        <f>SUM($H$32:H44)</f>
+        <v>69502.0</v>
+      </c>
+      <c r="K44" s="0" t="n">
+        <f>SUM($I$32:I44)</f>
+        <v>901.0</v>
+      </c>
+      <c r="L44" t="n">
+        <v>120.0</v>
+      </c>
+    </row>
+    <row r="45" ht="15.0" customHeight="true">
+      <c r="A45" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C45" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <f>B45-C45</f>
+        <v>1.0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>1966.0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1964.0</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <f>E45-F45</f>
+        <v>2.0</v>
+      </c>
+      <c r="H45" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="I45" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J45" s="0" t="n">
+        <f>SUM($H$32:H45)</f>
+        <v>69509.0</v>
+      </c>
+      <c r="K45" s="0" t="n">
+        <f>SUM($I$32:I45)</f>
+        <v>902.0</v>
+      </c>
+      <c r="L45" t="n">
+        <v>163.0</v>
+      </c>
+    </row>
+    <row r="46" ht="15.0" customHeight="true">
+      <c r="A46" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C46" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <f>B46-C46</f>
+        <v>0.0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>1964.0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>1964.0</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <f>E46-F46</f>
+        <v>0.0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J46" s="0" t="n">
+        <f>SUM($H$32:H46)</f>
+        <v>69511.0</v>
+      </c>
+      <c r="K46" s="0" t="n">
+        <f>SUM($I$32:I46)</f>
+        <v>902.0</v>
+      </c>
+      <c r="L46" t="n">
+        <v>22.0</v>
+      </c>
+    </row>
+    <row r="47" ht="15.0" customHeight="true">
+      <c r="A47" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <f>B47-C47</f>
+        <v>0.0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>1964.0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>1964.0</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <f>E47-F47</f>
+        <v>0.0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J47" s="0" t="n">
+        <f>SUM($H$32:H47)</f>
+        <v>69511.0</v>
+      </c>
+      <c r="K47" s="0" t="n">
+        <f>SUM($I$32:I47)</f>
+        <v>902.0</v>
+      </c>
+      <c r="L47" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
VM run GDDrec for chart_2
</commit_message>
<xml_diff>
--- a/stats/Statistics.xlsx
+++ b/stats/Statistics.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lubo9\Desktop\Workspace\ddminj\stats\"/>
     </mc:Choice>
@@ -15,10 +15,11 @@
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
     <sheet name="Template" sheetId="1" r:id="rId2"/>
+    <sheet name="GDDrec_chart_2_b_20230615_11275" r:id="rId7" sheetId="3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>Execution Time (ms)</t>
   </si>
@@ -175,12 +176,46 @@
   </si>
   <si>
     <t>Average run size</t>
+  </si>
+  <si>
+    <t>chart_2_b</t>
+  </si>
+  <si>
+    <t>/home/lukasbosshart/workspace/defects4j/bugs/chart_2_b</t>
+  </si>
+  <si>
+    <t>source/</t>
+  </si>
+  <si>
+    <t>tests/</t>
+  </si>
+  <si>
+    <t>org.jfree.data.general.junit.DatasetUtilitiesTests#testBug2849731_2</t>
+  </si>
+  <si>
+    <t>java.lang.NullPointerException</t>
+  </si>
+  <si>
+    <t>IN_MEMORY</t>
+  </si>
+  <si>
+    <t>INFO</t>
+  </si>
+  <si>
+    <t>GDDrec</t>
+  </si>
+  <si>
+    <t>0-0</t>
+  </si>
+  <si>
+    <t>0-1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -775,6 +810,423 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EB3A-4356-BAD6-BBDF08267E46}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1714316624"/>
+        <c:axId val="1714318064"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1714316624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># compiler calls</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1714318064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1714318064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># fragments</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1714316624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t># of fragments after # of compiler calls</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Template!$F$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Result</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>GDDrec_chart_2_b_20230615_11275!$J$32:$J$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>GDDrec_chart_2_b_20230615_11275!$F$32:$F$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1691,6 +2143,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1996,7 +2491,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2024,14 +2519,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="39.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="30.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2143,9 +2638,9 @@
       <c r="C20" t="s">
         <v>35</v>
       </c>
-      <c r="D20">
+      <c r="D20" t="n">
         <f>COUNTA(A32:A32)</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2268,21 +2763,21 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32"/>
-      <c r="D32">
+      <c r="D32" t="n">
         <f>B32-C32</f>
-        <v>0</v>
-      </c>
-      <c r="G32">
+        <v>0.0</v>
+      </c>
+      <c r="G32" t="n">
         <f>E32-F32</f>
-        <v>0</v>
-      </c>
-      <c r="J32">
+        <v>0.0</v>
+      </c>
+      <c r="J32" t="n">
         <f>SUM($H$32:H32)</f>
-        <v>0</v>
-      </c>
-      <c r="K32">
+        <v>0.0</v>
+      </c>
+      <c r="K32" t="n">
         <f>SUM($I$32:I32)</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2314,4 +2809,425 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0AC2FFA-B2F6-4AE0-A9AF-E35D0D2B929E}">
+  <dimension ref="A1:M33"/>
+  <sheetViews>
+    <sheetView tabSelected="false" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="39.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="30.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="n">
+        <v>407987.0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="n">
+        <f>COUNTA(A32:A33)</f>
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="n">
+        <v>6838600.0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="n">
+        <f>B27/D20</f>
+        <v>5858.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="n">
+        <v>227306.0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="4" t="n">
+        <f>(B20-B23)/B20</f>
+        <v>0.03445207812994042</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="n">
+        <v>393931.0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="4" t="n">
+        <f>D22/D20</f>
+        <v>0.01722603906497021</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="n">
+        <v>3026209.0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="str">
+        <f>TEXT(B26/86400000,"hh:mm:ss.000")</f>
+        <v>04:00:09.572</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="n">
+        <v>108815.0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" t="n">
+        <f>AVERAGE(B32:B33)</f>
+        <v>332.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1.4409572E7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="n">
+        <v>11716.0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="n">
+        <v>87.0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" t="n">
+        <v>654.0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>611.0</v>
+      </c>
+      <c r="D32" t="n">
+        <f>B32-C32</f>
+        <v>43.0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>407987.0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>393931.0</v>
+      </c>
+      <c r="G32" t="n">
+        <f>E32-F32</f>
+        <v>14056.0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>11716.0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>87.0</v>
+      </c>
+      <c r="J32" t="n">
+        <f>SUM($H$32:H32)</f>
+        <v>11716.0</v>
+      </c>
+      <c r="K32" t="n">
+        <f>SUM($I$32:I32)</f>
+        <v>87.0</v>
+      </c>
+      <c r="L32" t="n">
+        <v>1.37544E7</v>
+      </c>
+      <c r="M32" t="n">
+        <v>1.4408143E7</v>
+      </c>
+    </row>
+    <row r="33" ht="15.0" customHeight="true">
+      <c r="A33" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <f>B33-C33</f>
+        <v>0.0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>393931.0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>393931.0</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <f>E33-F33</f>
+        <v>0.0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <f>SUM($H$32:H33)</f>
+        <v>11716.0</v>
+      </c>
+      <c r="K33" s="0" t="n">
+        <f>SUM($I$32:I33)</f>
+        <v>87.0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>1.4408246E7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
VM run HDDrec for chart_2
</commit_message>
<xml_diff>
--- a/stats/Statistics.xlsx
+++ b/stats/Statistics.xlsx
@@ -16,6 +16,7 @@
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
     <sheet name="Template" sheetId="1" r:id="rId2"/>
     <sheet name="GDDrec_chart_2_b_20230615_11275" r:id="rId7" sheetId="3"/>
+    <sheet name="HDDrec_chart_2_b_20230615_15281" r:id="rId8" sheetId="4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
   <si>
     <t>Execution Time (ms)</t>
   </si>
@@ -209,6 +210,9 @@
   </si>
   <si>
     <t>0-1</t>
+  </si>
+  <si>
+    <t>HDDrec</t>
   </si>
 </sst>
 </file>
@@ -1514,6 +1518,423 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t># of fragments after # of compiler calls</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Template!$F$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Result</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>HDDrec_chart_2_b_20230615_15281!$J$32:$J$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>HDDrec_chart_2_b_20230615_15281!$F$32:$F$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EB3A-4356-BAD6-BBDF08267E46}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1714316624"/>
+        <c:axId val="1714318064"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1714316624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># compiler calls</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1714318064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1714318064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># fragments</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1714316624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2186,6 +2607,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3230,4 +3694,380 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0AC2FFA-B2F6-4AE0-A9AF-E35D0D2B929E}">
+  <dimension ref="A1:M32"/>
+  <sheetViews>
+    <sheetView tabSelected="false" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="39.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="30.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="n">
+        <v>408643.0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="n">
+        <f>COUNTA(A32:A32)</f>
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="n">
+        <v>6838600.0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="n">
+        <f>B27/D20</f>
+        <v>5894.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="n">
+        <v>227306.0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="4" t="n">
+        <f>(B20-B23)/B20</f>
+        <v>0.02850409770875801</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="n">
+        <v>396995.0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="4" t="n">
+        <f>D22/D20</f>
+        <v>0.02850409770875801</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="n">
+        <v>3044039.0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="str">
+        <f>TEXT(B26/86400000,"hh:mm:ss.000")</f>
+        <v>04:00:07.533</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="n">
+        <v>109471.0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" t="n">
+        <f>AVERAGE(B32:B32)</f>
+        <v>654.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1.4407533E7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="n">
+        <v>5894.0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="n">
+        <v>49.0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" t="n">
+        <v>654.0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>623.0</v>
+      </c>
+      <c r="D32" t="n">
+        <f>B32-C32</f>
+        <v>31.0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>408643.0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>396995.0</v>
+      </c>
+      <c r="G32" t="n">
+        <f>E32-F32</f>
+        <v>11648.0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>5894.0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="J32" t="n">
+        <f>SUM($H$32:H32)</f>
+        <v>5894.0</v>
+      </c>
+      <c r="K32" t="n">
+        <f>SUM($I$32:I32)</f>
+        <v>49.0</v>
+      </c>
+      <c r="L32" t="n">
+        <v>1.4389233E7</v>
+      </c>
+      <c r="M32" t="n">
+        <v>1.4406707E7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
VM run GDD for chart_2
</commit_message>
<xml_diff>
--- a/stats/Statistics.xlsx
+++ b/stats/Statistics.xlsx
@@ -17,6 +17,7 @@
     <sheet name="Template" sheetId="1" r:id="rId2"/>
     <sheet name="GDDrec_chart_2_b_20230615_11275" r:id="rId7" sheetId="3"/>
     <sheet name="HDDrec_chart_2_b_20230615_15281" r:id="rId8" sheetId="4"/>
+    <sheet name="GDD_chart_2_b_20230615_192837" r:id="rId9" sheetId="5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
   <si>
     <t>Execution Time (ms)</t>
   </si>
@@ -213,6 +214,9 @@
   </si>
   <si>
     <t>HDDrec</t>
+  </si>
+  <si>
+    <t>GDD</t>
   </si>
 </sst>
 </file>
@@ -1935,6 +1939,423 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t># of fragments after # of compiler calls</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Template!$F$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Result</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>GDD_chart_2_b_20230615_192837!$J$32:$J$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>GDD_chart_2_b_20230615_192837!$F$32:$F$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EB3A-4356-BAD6-BBDF08267E46}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1714316624"/>
+        <c:axId val="1714318064"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1714316624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># compiler calls</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1714318064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1714318064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># fragments</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1714316624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2650,6 +3071,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4070,4 +4534,425 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0AC2FFA-B2F6-4AE0-A9AF-E35D0D2B929E}">
+  <dimension ref="A1:M33"/>
+  <sheetViews>
+    <sheetView tabSelected="false" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="39.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="30.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="n">
+        <v>407987.0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="n">
+        <f>COUNTA(A32:A33)</f>
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="n">
+        <v>6838600.0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="n">
+        <f>B27/D20</f>
+        <v>6028.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="n">
+        <v>227306.0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="4" t="n">
+        <f>(B20-B23)/B20</f>
+        <v>0.031969155879966765</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="n">
+        <v>394944.0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="4" t="n">
+        <f>D22/D20</f>
+        <v>0.015984577939983383</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="n">
+        <v>3033616.0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="str">
+        <f>TEXT(B26/86400000,"hh:mm:ss.000")</f>
+        <v>04:00:09.141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="n">
+        <v>109042.0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" t="n">
+        <f>AVERAGE(B32:B33)</f>
+        <v>3671.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1.4409141E7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="n">
+        <v>12057.0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="n">
+        <v>101.0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" t="n">
+        <v>654.0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>614.0</v>
+      </c>
+      <c r="D32" t="n">
+        <f>B32-C32</f>
+        <v>40.0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>407987.0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>394944.0</v>
+      </c>
+      <c r="G32" t="n">
+        <f>E32-F32</f>
+        <v>13043.0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>12057.0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>101.0</v>
+      </c>
+      <c r="J32" t="n">
+        <f>SUM($H$32:H32)</f>
+        <v>12057.0</v>
+      </c>
+      <c r="K32" t="n">
+        <f>SUM($I$32:I32)</f>
+        <v>101.0</v>
+      </c>
+      <c r="L32" t="n">
+        <v>1.3800833E7</v>
+      </c>
+      <c r="M32" t="n">
+        <v>1.4407067E7</v>
+      </c>
+    </row>
+    <row r="33" ht="15.0" customHeight="true">
+      <c r="A33" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" t="n">
+        <v>6688.0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>6688.0</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <f>B33-C33</f>
+        <v>0.0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>394944.0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>394944.0</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <f>E33-F33</f>
+        <v>0.0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <f>SUM($H$32:H33)</f>
+        <v>12057.0</v>
+      </c>
+      <c r="K33" s="0" t="n">
+        <f>SUM($I$32:I33)</f>
+        <v>101.0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>1194.0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>1.4408261E7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
VM run HDD for chart_2
</commit_message>
<xml_diff>
--- a/stats/Statistics.xlsx
+++ b/stats/Statistics.xlsx
@@ -18,6 +18,7 @@
     <sheet name="GDDrec_chart_2_b_20230615_11275" r:id="rId7" sheetId="3"/>
     <sheet name="HDDrec_chart_2_b_20230615_15281" r:id="rId8" sheetId="4"/>
     <sheet name="GDD_chart_2_b_20230615_192837" r:id="rId9" sheetId="5"/>
+    <sheet name="HDD_chart_2_b_20230615_232859" r:id="rId10" sheetId="6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="60">
   <si>
     <t>Execution Time (ms)</t>
   </si>
@@ -217,6 +218,9 @@
   </si>
   <si>
     <t>GDD</t>
+  </si>
+  <si>
+    <t>HDD</t>
   </si>
 </sst>
 </file>
@@ -2356,6 +2360,423 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t># of fragments after # of compiler calls</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Template!$F$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Result</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>HDD_chart_2_b_20230615_232859!$J$32:$J$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>HDD_chart_2_b_20230615_232859!$F$32:$F$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EB3A-4356-BAD6-BBDF08267E46}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1714316624"/>
+        <c:axId val="1714318064"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1714316624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># compiler calls</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1714318064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1714318064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># fragments</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1714316624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3114,6 +3535,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4955,4 +5419,380 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0AC2FFA-B2F6-4AE0-A9AF-E35D0D2B929E}">
+  <dimension ref="A1:M32"/>
+  <sheetViews>
+    <sheetView tabSelected="false" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="39.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="30.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="n">
+        <v>408643.0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="n">
+        <f>COUNTA(A32:A32)</f>
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="n">
+        <v>6838600.0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="n">
+        <f>B27/D20</f>
+        <v>5752.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="n">
+        <v>227306.0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="4" t="n">
+        <f>(B20-B23)/B20</f>
+        <v>0.02850409770875801</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="n">
+        <v>396995.0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="4" t="n">
+        <f>D22/D20</f>
+        <v>0.02850409770875801</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="n">
+        <v>3044039.0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="str">
+        <f>TEXT(B26/86400000,"hh:mm:ss.000")</f>
+        <v>04:00:32.171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="n">
+        <v>109471.0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" t="n">
+        <f>AVERAGE(B32:B32)</f>
+        <v>654.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1.4432171E7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="n">
+        <v>5752.0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="n">
+        <v>48.0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" t="n">
+        <v>654.0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>623.0</v>
+      </c>
+      <c r="D32" t="n">
+        <f>B32-C32</f>
+        <v>31.0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>408643.0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>396995.0</v>
+      </c>
+      <c r="G32" t="n">
+        <f>E32-F32</f>
+        <v>11648.0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>5752.0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="J32" t="n">
+        <f>SUM($H$32:H32)</f>
+        <v>5752.0</v>
+      </c>
+      <c r="K32" t="n">
+        <f>SUM($I$32:I32)</f>
+        <v>48.0</v>
+      </c>
+      <c r="L32" t="n">
+        <v>1.4417275E7</v>
+      </c>
+      <c r="M32" t="n">
+        <v>1.4430983E7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
VM run CodeLine for chart_2
</commit_message>
<xml_diff>
--- a/stats/Statistics.xlsx
+++ b/stats/Statistics.xlsx
@@ -19,6 +19,7 @@
     <sheet name="HDDrec_chart_2_b_20230615_15281" r:id="rId8" sheetId="4"/>
     <sheet name="GDD_chart_2_b_20230615_192837" r:id="rId9" sheetId="5"/>
     <sheet name="HDD_chart_2_b_20230615_232859" r:id="rId10" sheetId="6"/>
+    <sheet name="CodeLine__2__20230616_032944" r:id="rId11" sheetId="7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="62">
   <si>
     <t>Execution Time (ms)</t>
   </si>
@@ -221,6 +222,12 @@
   </si>
   <si>
     <t>HDD</t>
+  </si>
+  <si>
+    <t>CodeLine</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -2777,6 +2784,423 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t># of fragments after # of compiler calls</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Template!$F$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Result</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>CodeLine__2__20230616_032944!$J$32:$J$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>CodeLine__2__20230616_032944!$F$32:$F$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EB3A-4356-BAD6-BBDF08267E46}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1714316624"/>
+        <c:axId val="1714318064"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1714316624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># compiler calls</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1714318064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1714318064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># fragments</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1714316624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3578,6 +4002,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5795,4 +6262,380 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0AC2FFA-B2F6-4AE0-A9AF-E35D0D2B929E}">
+  <dimension ref="A1:M32"/>
+  <sheetViews>
+    <sheetView tabSelected="false" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="39.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="30.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="n">
+        <v>227306.0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="n">
+        <f>COUNTA(A32:A32)</f>
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="n">
+        <v>6838600.0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="n">
+        <f>B27/D20</f>
+        <v>1216.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="n">
+        <v>227306.0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="4" t="n">
+        <f>(B20-B23)/B20</f>
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="n">
+        <v>227306.0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="4" t="n">
+        <f>D22/D20</f>
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="n">
+        <v>6838611.0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="str">
+        <f>TEXT(B26/86400000,"hh:mm:ss.000")</f>
+        <v>04:31:05.693</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="n">
+        <v>227306.0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" t="n">
+        <f>AVERAGE(B32:B32)</f>
+        <v>227306.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1.6265693E7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1216.0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" t="n">
+        <v>227306.0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>227306.0</v>
+      </c>
+      <c r="D32" t="n">
+        <f>B32-C32</f>
+        <v>0.0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>227306.0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>227306.0</v>
+      </c>
+      <c r="G32" t="n">
+        <f>E32-F32</f>
+        <v>0.0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1216.0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J32" t="n">
+        <f>SUM($H$32:H32)</f>
+        <v>1216.0</v>
+      </c>
+      <c r="K32" t="n">
+        <f>SUM($I$32:I32)</f>
+        <v>1.0</v>
+      </c>
+      <c r="L32" t="n">
+        <v>1.6261622E7</v>
+      </c>
+      <c r="M32" t="n">
+        <v>1.6265071E7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>